<commit_message>
Country Registration Form -new person creation. roles(chw->chp)
</commit_message>
<xml_diff>
--- a/forms/contact/county-create.xlsx
+++ b/forms/contact/county-create.xlsx
@@ -907,10 +907,10 @@
     <t>roles</t>
   </si>
   <si>
-    <t>chw</t>
-  </si>
-  <si>
-    <t>CHW</t>
+    <t>chp</t>
+  </si>
+  <si>
+    <t>CHP</t>
   </si>
   <si>
     <t>सामुदायिक स्वास्थ्य कर्मी</t>
@@ -928,10 +928,10 @@
     <t>ASC</t>
   </si>
   <si>
-    <t>chw_supervisor</t>
-  </si>
-  <si>
-    <t>CHW Supervisor</t>
+    <t>chp_supervisor</t>
+  </si>
+  <si>
+    <t>CHP Supervisor</t>
   </si>
   <si>
     <t>सामुदायिक स्वास्थ्य कर्मी के मैनेजर</t>
@@ -1225,8 +1225,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
@@ -1279,14 +1279,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1294,19 +1286,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1320,14 +1317,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1347,6 +1337,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -1355,39 +1352,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1399,8 +1368,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1414,10 +1391,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1490,7 +1490,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1502,61 +1610,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1574,48 +1628,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1628,37 +1640,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1670,7 +1664,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,35 +1684,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1764,6 +1740,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1773,145 +1775,143 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="14" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
@@ -2184,7 +2184,7 @@
   <dimension ref="A1:AR76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -6572,7 +6572,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A22" sqref="$A22:$XFD25"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.437037037037" defaultRowHeight="15"/>
@@ -7447,7 +7447,7 @@
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">TEXT(NOW(),"yyyy-mm-dd_HH-MM")</f>
-        <v>2024-03-28 14-55</v>
+        <v>2024-04-16 8-56</v>
       </c>
       <c r="D2" t="s">
         <v>397</v>

</xml_diff>

<commit_message>
Update of the edit forms to match the create forms
</commit_message>
<xml_diff>
--- a/forms/contact/county-create.xlsx
+++ b/forms/contact/county-create.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12930"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="401">
   <si>
     <t>type</t>
   </si>
@@ -698,6 +698,12 @@
   </si>
   <si>
     <t>selected(${available_health_facilities},'yes')</t>
+  </si>
+  <si>
+    <t>.&gt;=1</t>
+  </si>
+  <si>
+    <t>It must be greater than 1</t>
   </si>
   <si>
     <t>select_one yes_no_natural_park</t>
@@ -1225,9 +1231,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1273,6 +1279,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1289,13 +1307,77 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1310,84 +1392,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1401,13 +1414,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1415,7 +1421,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1490,7 +1496,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1502,7 +1520,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1520,7 +1538,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1532,7 +1550,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1544,55 +1640,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1610,67 +1670,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1711,8 +1717,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1776,145 +1782,145 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2183,12 +2189,12 @@
   <sheetPr/>
   <dimension ref="A1:AR76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="K52" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.437037037037" defaultRowHeight="15"/>
@@ -5819,8 +5825,12 @@
       </c>
       <c r="L63" s="29"/>
       <c r="M63" s="29"/>
-      <c r="N63" s="29"/>
-      <c r="O63" s="31"/>
+      <c r="N63" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="O63" s="29" t="s">
+        <v>227</v>
+      </c>
       <c r="P63" s="29"/>
       <c r="Q63" s="29"/>
       <c r="R63" s="29"/>
@@ -5853,13 +5863,13 @@
     </row>
     <row r="64" ht="14.25" customHeight="1" spans="1:44">
       <c r="A64" s="28" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="29"/>
@@ -5910,10 +5920,10 @@
         <v>124</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29"/>
@@ -5923,12 +5933,16 @@
       <c r="I65" s="29"/>
       <c r="J65" s="29"/>
       <c r="K65" s="29" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="L65" s="29"/>
       <c r="M65" s="29"/>
-      <c r="N65" s="29"/>
-      <c r="O65" s="29"/>
+      <c r="N65" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="O65" s="29" t="s">
+        <v>227</v>
+      </c>
       <c r="P65" s="29"/>
       <c r="Q65" s="29"/>
       <c r="R65" s="29"/>
@@ -5961,13 +5975,13 @@
     </row>
     <row r="66" ht="14.25" customHeight="1" spans="1:44">
       <c r="A66" s="28" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29"/>
@@ -5977,7 +5991,7 @@
       <c r="I66" s="29"/>
       <c r="J66" s="29"/>
       <c r="K66" s="29" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="L66" s="29"/>
       <c r="M66" s="29"/>
@@ -6030,7 +6044,7 @@
         <v>188</v>
       </c>
       <c r="F67" s="29" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G67" s="30" t="s">
         <v>190</v>
@@ -6160,7 +6174,7 @@
       <c r="N69" s="29"/>
       <c r="O69" s="29"/>
       <c r="P69" s="29" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="Q69" s="29"/>
       <c r="R69" s="29"/>
@@ -6196,7 +6210,7 @@
         <v>59</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C70" s="29"/>
       <c r="D70" s="29"/>
@@ -6212,7 +6226,7 @@
       <c r="N70" s="29"/>
       <c r="O70" s="29"/>
       <c r="P70" s="29" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Q70" s="29"/>
       <c r="R70" s="29"/>
@@ -6571,8 +6585,8 @@
   <sheetPr/>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A21" sqref="$A21:$XFD25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.437037037037" defaultRowHeight="15"/>
@@ -6591,7 +6605,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -6620,110 +6634,110 @@
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:9">
       <c r="A3" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:9">
       <c r="A4" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:9">
       <c r="A5" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="24" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:9">
@@ -6731,26 +6745,26 @@
         <v>86</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="24" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:9">
@@ -6758,26 +6772,26 @@
         <v>86</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="24" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" spans="1:9">
@@ -6785,37 +6799,37 @@
         <v>86</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="24" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:9">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="21"/>
@@ -6826,218 +6840,218 @@
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:9">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="24" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:9">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="24" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:9">
       <c r="A12" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F12" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>313</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>311</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="24" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" spans="1:9">
       <c r="A13" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="24" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:9">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B14" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C14" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="24" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:9">
       <c r="A15" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="F15" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>332</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>330</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="24" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1" spans="1:9">
       <c r="A16" s="5" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>214</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:9">
       <c r="A17" s="5" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="24" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:9">
@@ -7045,26 +7059,26 @@
         <v>72</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="24" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:9">
@@ -7072,26 +7086,26 @@
         <v>72</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="24" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1" spans="1:9">
@@ -7099,26 +7113,26 @@
         <v>72</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="F20" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="G20" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>358</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="24" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" customFormat="1" ht="14.25" customHeight="1" spans="1:9">
@@ -7126,26 +7140,26 @@
         <v>83</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="24" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" customFormat="1" ht="14.25" customHeight="1" spans="1:9">
@@ -7153,26 +7167,26 @@
         <v>83</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="G22" s="19" t="s">
         <v>369</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>365</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>367</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="24" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:9">
@@ -7180,26 +7194,26 @@
         <v>83</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="24" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:9">
@@ -7207,26 +7221,26 @@
         <v>83</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="24" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1" spans="1:9">
@@ -7234,31 +7248,31 @@
         <v>83</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="24" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="1:9">
       <c r="A26" s="12" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>1</v>
@@ -7285,61 +7299,61 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>47</v>
@@ -7348,25 +7362,25 @@
         <v>47</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>104</v>
@@ -7375,20 +7389,20 @@
         <v>104</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H30" s="20"/>
       <c r="I30" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -7422,38 +7436,38 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:5">
       <c r="A2" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">TEXT(NOW(),"yyyy-mm-dd_HH-MM")</f>
-        <v>2024-04-17 12-46</v>
+        <v>2024-05-02 10-42</v>
       </c>
       <c r="D2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>

</xml_diff>